<commit_message>
run methods in parallel
</commit_message>
<xml_diff>
--- a/TOU_Default1/data/TestData.xlsx
+++ b/TOU_Default1/data/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908026B0-ACB4-46A7-B8AB-A8A3C75A082A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061837D8-3C89-48F8-94C5-5CE554CAA982}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -34,9 +34,6 @@
     <t>editEmployeeDetails</t>
   </si>
   <si>
-    <t>verifyListBox</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -47,6 +44,12 @@
   </si>
   <si>
     <t>Giana</t>
+  </si>
+  <si>
+    <t>launchOrangeHRM</t>
+  </si>
+  <si>
+    <t>john</t>
   </si>
 </sst>
 </file>
@@ -367,18 +370,18 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -389,26 +392,35 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added one more TC3
</commit_message>
<xml_diff>
--- a/TOU_Default1/data/TestData.xlsx
+++ b/TOU_Default1/data/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061837D8-3C89-48F8-94C5-5CE554CAA982}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEF16EB-C7C8-4CF0-A24F-6DCAE1749E31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>john</t>
+  </si>
+  <si>
+    <t>forgotPassword</t>
   </si>
 </sst>
 </file>
@@ -367,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,6 +426,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>